<commit_message>
Seems like pretty good results from changing F bounds
</commit_message>
<xml_diff>
--- a/AIC9parameters_hptoolbox_moredata.xlsx
+++ b/AIC9parameters_hptoolbox_moredata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C2517BD-DE08-4D88-A15D-F0311C1FAA28}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD9DABC0-9FD8-415E-B617-497CA11B9F88}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11325" xr2:uid="{39B4C127-F51D-4565-9B09-D204C61B9351}"/>
+    <workbookView xWindow="1440" yWindow="1032" windowWidth="21600" windowHeight="11328" xr2:uid="{39B4C127-F51D-4565-9B09-D204C61B9351}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -387,244 +387,244 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>2462.8448573775845</v>
+        <v>2504.3641967919812</v>
       </c>
       <c r="B1">
-        <v>1623.1567450532016</v>
+        <v>1675.4831224905172</v>
       </c>
       <c r="C1">
-        <v>1669.587306250352</v>
+        <v>1659.1742236099808</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2286.4378582848854</v>
+        <v>2263.2649178670267</v>
       </c>
       <c r="B2">
-        <v>1565.8373548998079</v>
+        <v>1537.5656129537554</v>
       </c>
       <c r="C2">
-        <v>1532.9228662751209</v>
+        <v>1393.3171188274771</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2558.4526913863224</v>
+        <v>2560.3680356546965</v>
       </c>
       <c r="B3">
-        <v>1802.9820621229946</v>
+        <v>1740.678815942545</v>
       </c>
       <c r="C3">
-        <v>1690.5994019799068</v>
+        <v>1579.3443776225236</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2541.0494842846788</v>
+        <v>2495.9981556247999</v>
       </c>
       <c r="B4">
-        <v>1942.9487479649179</v>
+        <v>1913.0014038613795</v>
       </c>
       <c r="C4">
-        <v>2003.7073007303677</v>
+        <v>1950.7277354949008</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2540.5942711499938</v>
+        <v>2528.8694636736568</v>
       </c>
       <c r="B5">
-        <v>1997.3880411242792</v>
+        <v>1742.3270368293149</v>
       </c>
       <c r="C5">
-        <v>2040.7628848173006</v>
+        <v>1784.7568909152653</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2532.6044642876955</v>
+        <v>2480.0523703440967</v>
       </c>
       <c r="B6">
-        <v>1876.7544258655212</v>
+        <v>1850.3730377169611</v>
       </c>
       <c r="C6">
-        <v>1999.1684512162235</v>
+        <v>1931.0848430119481</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2325.1604081261567</v>
+        <v>2397.2088800503925</v>
       </c>
       <c r="B7">
-        <v>1762.8219710754731</v>
+        <v>1848.4300944536446</v>
       </c>
       <c r="C7">
-        <v>1635.1671999331111</v>
+        <v>1675.668040406772</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2427.6950325843745</v>
+        <v>2467.9969983108795</v>
       </c>
       <c r="B8">
-        <v>1881.8645114639951</v>
+        <v>1930.0320208708331</v>
       </c>
       <c r="C8">
-        <v>1754.7904942225448</v>
+        <v>1785.2136052421129</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2648.4487534981058</v>
+        <v>2643.8787318127324</v>
       </c>
       <c r="B9">
-        <v>2063.7700731963514</v>
+        <v>1963.5067209681306</v>
       </c>
       <c r="C9">
-        <v>1896.9360911440497</v>
+        <v>1680.4583613843849</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2485.6040968258926</v>
+        <v>2394.9101549394882</v>
       </c>
       <c r="B10">
-        <v>1537.1807659240974</v>
+        <v>1520.9883557933742</v>
       </c>
       <c r="C10">
-        <v>1442.1296088642237</v>
+        <v>1428.5183673137938</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>2175.6124502111961</v>
+        <v>2163.0420355061924</v>
       </c>
       <c r="B11">
-        <v>1642.223316563649</v>
+        <v>1575.4241743753942</v>
       </c>
       <c r="C11">
-        <v>1625.8576302467475</v>
+        <v>1407.2608779610723</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>2830.2849258372607</v>
+        <v>2770.6265500970344</v>
       </c>
       <c r="B12">
-        <v>2419.8290592433436</v>
+        <v>2207.4257872533763</v>
       </c>
       <c r="C12">
-        <v>2361.9699099525315</v>
+        <v>1916.0906809257067</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>2580.4055975139845</v>
+        <v>2528.2387480558714</v>
       </c>
       <c r="B13">
-        <v>2039.8559365770425</v>
+        <v>1947.5474619142117</v>
       </c>
       <c r="C13">
-        <v>1736.7142084625405</v>
+        <v>1749.6306059708488</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>2566.681798017014</v>
+        <v>2609.7083426384261</v>
       </c>
       <c r="B14">
-        <v>1970.8229598244188</v>
+        <v>2019.1228183797468</v>
       </c>
       <c r="C14">
-        <v>1729.7759258115523</v>
+        <v>1756.8907062203525</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>2675.7591696896948</v>
+        <v>2503.2255475334637</v>
       </c>
       <c r="B15">
-        <v>2278.6202922031093</v>
+        <v>2051.809549640262</v>
       </c>
       <c r="C15">
-        <v>2267.0569566136055</v>
+        <v>1832.9655400561949</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>2588.3505586700676</v>
+        <v>2592.375598703285</v>
       </c>
       <c r="B16">
-        <v>1832.3279750711042</v>
+        <v>1804.6455680313004</v>
       </c>
       <c r="C16">
-        <v>1479.2456770422921</v>
+        <v>1530.1185850923541</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>2407.3416567476406</v>
+        <v>2356.8601578997373</v>
       </c>
       <c r="B17">
-        <v>1834.7039704285885</v>
+        <v>1814.1810148436214</v>
       </c>
       <c r="C17">
-        <v>1771.1796536663489</v>
+        <v>1709.7047242962224</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>2675.0265898774014</v>
+        <v>2615.4902880995196</v>
       </c>
       <c r="B18">
-        <v>2306.0901010097209</v>
+        <v>2163.225143496114</v>
       </c>
       <c r="C18">
-        <v>2363.8072009952193</v>
+        <v>2077.8195710672057</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>2016.5354504077682</v>
+        <v>2011.2280643505962</v>
       </c>
       <c r="B19">
-        <v>2025.2006132386789</v>
+        <v>2033.9321272375284</v>
       </c>
       <c r="C19">
-        <v>1980.3712985764628</v>
+        <v>1981.0696108332579</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>2565.9191954314083</v>
+        <v>2576.2845510916013</v>
       </c>
       <c r="B20">
-        <v>1983.5459444064861</v>
+        <v>1981.3683885098346</v>
       </c>
       <c r="C20">
-        <v>1866.3437936470029</v>
+        <v>1870.0663422816451</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>2715.1785561517936</v>
+        <v>2713.0801993379068</v>
       </c>
       <c r="B21">
-        <v>2158.0273766418918</v>
+        <v>2020.8570131593781</v>
       </c>
       <c r="C21">
-        <v>2176.6791952365493</v>
+        <v>1980.6742669114219</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>2630.1522641369579</v>
+        <v>2569.5114392622113</v>
       </c>
       <c r="B22">
-        <v>2192.2515050924062</v>
+        <v>1982.4395818578371</v>
       </c>
       <c r="C22">
-        <v>2202.3474444735239</v>
+        <v>1731.9556707015938</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
kMCT4 trend is back, definitely a result of FL bounds
</commit_message>
<xml_diff>
--- a/AIC9parameters_hptoolbox_moredata.xlsx
+++ b/AIC9parameters_hptoolbox_moredata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD9DABC0-9FD8-415E-B617-497CA11B9F88}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A38CA9-851C-4023-9E68-EE30FBA7B0ED}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1440" yWindow="1032" windowWidth="21600" windowHeight="11328" xr2:uid="{39B4C127-F51D-4565-9B09-D204C61B9351}"/>
   </bookViews>
@@ -387,244 +387,244 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>2504.3641967919812</v>
+        <v>2504.364414539994</v>
       </c>
       <c r="B1">
-        <v>1675.4831224905172</v>
+        <v>1675.5675376436604</v>
       </c>
       <c r="C1">
-        <v>1659.1742236099808</v>
+        <v>1659.1065227383422</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2263.2649178670267</v>
+        <v>2263.2649011438675</v>
       </c>
       <c r="B2">
-        <v>1537.5656129537554</v>
+        <v>1537.5762282943956</v>
       </c>
       <c r="C2">
-        <v>1393.3171188274771</v>
+        <v>1393.3778585627351</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2560.3680356546965</v>
+        <v>2560.3680356085983</v>
       </c>
       <c r="B3">
-        <v>1740.678815942545</v>
+        <v>1740.3097987834262</v>
       </c>
       <c r="C3">
-        <v>1579.3443776225236</v>
+        <v>1583.9747961737785</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2495.9981556247999</v>
+        <v>2495.9915444752205</v>
       </c>
       <c r="B4">
-        <v>1913.0014038613795</v>
+        <v>1913.4487934162717</v>
       </c>
       <c r="C4">
-        <v>1950.7277354949008</v>
+        <v>1951.9452111165515</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2528.8694636736568</v>
+        <v>2528.80384513526</v>
       </c>
       <c r="B5">
-        <v>1742.3270368293149</v>
+        <v>1753.0003849402135</v>
       </c>
       <c r="C5">
-        <v>1784.7568909152653</v>
+        <v>1754.546258168725</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2480.0523703440967</v>
+        <v>2480.0509760227787</v>
       </c>
       <c r="B6">
-        <v>1850.3730377169611</v>
+        <v>1850.4755988030256</v>
       </c>
       <c r="C6">
-        <v>1931.0848430119481</v>
+        <v>1931.3762670675633</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2397.2088800503925</v>
+        <v>2397.2088802092485</v>
       </c>
       <c r="B7">
-        <v>1848.4300944536446</v>
+        <v>1848.4300945850457</v>
       </c>
       <c r="C7">
-        <v>1675.668040406772</v>
+        <v>1675.6680969497306</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2467.9969983108795</v>
+        <v>2467.9969987293316</v>
       </c>
       <c r="B8">
-        <v>1930.0320208708331</v>
+        <v>1930.0304210380705</v>
       </c>
       <c r="C8">
-        <v>1785.2136052421129</v>
+        <v>1785.2202694457196</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2643.8787318127324</v>
+        <v>2643.9044689181596</v>
       </c>
       <c r="B9">
-        <v>1963.5067209681306</v>
+        <v>1947.2351251927282</v>
       </c>
       <c r="C9">
-        <v>1680.4583613843849</v>
+        <v>1640.0636790523515</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2394.9101549394882</v>
+        <v>2394.9108734696329</v>
       </c>
       <c r="B10">
-        <v>1520.9883557933742</v>
+        <v>1511.42538690984</v>
       </c>
       <c r="C10">
-        <v>1428.5183673137938</v>
+        <v>1431.2601301716491</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>2163.0420355061924</v>
+        <v>2163.0420361799524</v>
       </c>
       <c r="B11">
-        <v>1575.4241743753942</v>
+        <v>1575.4238379800943</v>
       </c>
       <c r="C11">
-        <v>1407.2608779610723</v>
+        <v>1407.2614046763103</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>2770.6265500970344</v>
+        <v>2770.626449954108</v>
       </c>
       <c r="B12">
-        <v>2207.4257872533763</v>
+        <v>2193.8781744486687</v>
       </c>
       <c r="C12">
-        <v>1916.0906809257067</v>
+        <v>1875.1042057517848</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>2528.2387480558714</v>
+        <v>2528.2387490187198</v>
       </c>
       <c r="B13">
-        <v>1947.5474619142117</v>
+        <v>1947.5466896032067</v>
       </c>
       <c r="C13">
-        <v>1749.6306059708488</v>
+        <v>1749.6330418674784</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>2609.7083426384261</v>
+        <v>2609.7077573395409</v>
       </c>
       <c r="B14">
-        <v>2019.1228183797468</v>
+        <v>2018.5468677722945</v>
       </c>
       <c r="C14">
-        <v>1756.8907062203525</v>
+        <v>1759.5597087708768</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>2503.2255475334637</v>
+        <v>2503.2297760451011</v>
       </c>
       <c r="B15">
-        <v>2051.809549640262</v>
+        <v>2051.416880995745</v>
       </c>
       <c r="C15">
-        <v>1832.9655400561949</v>
+        <v>1833.0290098974242</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>2592.375598703285</v>
+        <v>2592.3768062015702</v>
       </c>
       <c r="B16">
-        <v>1804.6455680313004</v>
+        <v>1797.2456078784303</v>
       </c>
       <c r="C16">
-        <v>1530.1185850923541</v>
+        <v>1568.6528356072297</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>2356.8601578997373</v>
+        <v>2356.8601401089932</v>
       </c>
       <c r="B17">
-        <v>1814.1810148436214</v>
+        <v>1814.1836892896029</v>
       </c>
       <c r="C17">
-        <v>1709.7047242962224</v>
+        <v>1709.7092249325049</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>2615.4902880995196</v>
+        <v>2615.491122412915</v>
       </c>
       <c r="B18">
-        <v>2163.225143496114</v>
+        <v>2163.1508444250139</v>
       </c>
       <c r="C18">
-        <v>2077.8195710672057</v>
+        <v>2077.7982519417487</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>2011.2280643505962</v>
+        <v>2011.2261617487509</v>
       </c>
       <c r="B19">
-        <v>2033.9321272375284</v>
+        <v>2033.9335197896344</v>
       </c>
       <c r="C19">
-        <v>1981.0696108332579</v>
+        <v>1981.0698214975762</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>2576.2845510916013</v>
+        <v>2576.2845513363582</v>
       </c>
       <c r="B20">
-        <v>1981.3683885098346</v>
+        <v>1981.3717182002993</v>
       </c>
       <c r="C20">
-        <v>1870.0663422816451</v>
+        <v>1870.0558660754841</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>2713.0801993379068</v>
+        <v>2713.0802018334111</v>
       </c>
       <c r="B21">
-        <v>2020.8570131593781</v>
+        <v>2020.8570458484212</v>
       </c>
       <c r="C21">
-        <v>1980.6742669114219</v>
+        <v>1980.6742375270492</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>2569.5114392622113</v>
+        <v>2569.5114395448936</v>
       </c>
       <c r="B22">
-        <v>1982.4395818578371</v>
+        <v>1982.4411079456511</v>
       </c>
       <c r="C22">
-        <v>1731.9556707015938</v>
+        <v>1731.9360952080569</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Even with FL upper bound at 1.5, the KMCT4 trend is gone
</commit_message>
<xml_diff>
--- a/AIC9parameters_hptoolbox_moredata.xlsx
+++ b/AIC9parameters_hptoolbox_moredata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A38CA9-851C-4023-9E68-EE30FBA7B0ED}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E336764-4420-46F7-8A90-30CF35380784}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="1032" windowWidth="21600" windowHeight="11328" xr2:uid="{39B4C127-F51D-4565-9B09-D204C61B9351}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11325" xr2:uid="{39B4C127-F51D-4565-9B09-D204C61B9351}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -387,244 +387,244 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>2504.364414539994</v>
+        <v>2504.3641874528048</v>
       </c>
       <c r="B1">
-        <v>1675.5675376436604</v>
+        <v>1675.4872758024103</v>
       </c>
       <c r="C1">
-        <v>1659.1065227383422</v>
+        <v>1659.1694206955858</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2263.2649011438675</v>
+        <v>2263.2649304931097</v>
       </c>
       <c r="B2">
-        <v>1537.5762282943956</v>
+        <v>1537.5578724368795</v>
       </c>
       <c r="C2">
-        <v>1393.3778585627351</v>
+        <v>1393.2740556789715</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2560.3680356085983</v>
+        <v>2560.3680387196541</v>
       </c>
       <c r="B3">
-        <v>1740.3097987834262</v>
+        <v>1740.6137032078921</v>
       </c>
       <c r="C3">
-        <v>1583.9747961737785</v>
+        <v>1579.1404065201828</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2495.9915444752205</v>
+        <v>2495.9933054598469</v>
       </c>
       <c r="B4">
-        <v>1913.4487934162717</v>
+        <v>1913.3276998137765</v>
       </c>
       <c r="C4">
-        <v>1951.9452111165515</v>
+        <v>1951.620215286079</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2528.80384513526</v>
+        <v>2528.8045935782193</v>
       </c>
       <c r="B5">
-        <v>1753.0003849402135</v>
+        <v>1752.3685036322445</v>
       </c>
       <c r="C5">
-        <v>1754.546258168725</v>
+        <v>1755.617454012624</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2480.0509760227787</v>
+        <v>2480.0542736911661</v>
       </c>
       <c r="B6">
-        <v>1850.4755988030256</v>
+        <v>1850.23187819243</v>
       </c>
       <c r="C6">
-        <v>1931.3762670675633</v>
+        <v>1930.686298371365</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2397.2088802092485</v>
+        <v>2397.2088804141163</v>
       </c>
       <c r="B7">
-        <v>1848.4300945850457</v>
+        <v>1848.4313192171414</v>
       </c>
       <c r="C7">
-        <v>1675.6680969497306</v>
+        <v>1675.6626888020246</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2467.9969987293316</v>
+        <v>2467.9969994687162</v>
       </c>
       <c r="B8">
-        <v>1930.0304210380705</v>
+        <v>1930.0304952068079</v>
       </c>
       <c r="C8">
-        <v>1785.2202694457196</v>
+        <v>1785.2212237624467</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2643.9044689181596</v>
+        <v>2643.8787844459366</v>
       </c>
       <c r="B9">
-        <v>1947.2351251927282</v>
+        <v>1957.2149355131842</v>
       </c>
       <c r="C9">
-        <v>1640.0636790523515</v>
+        <v>1663.4754274722636</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2394.9108734696329</v>
+        <v>2394.9100079198947</v>
       </c>
       <c r="B10">
-        <v>1511.42538690984</v>
+        <v>1513.0137755996332</v>
       </c>
       <c r="C10">
-        <v>1431.2601301716491</v>
+        <v>1430.9226292086887</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>2163.0420361799524</v>
+        <v>2163.0420354858652</v>
       </c>
       <c r="B11">
-        <v>1575.4238379800943</v>
+        <v>1575.4241850871933</v>
       </c>
       <c r="C11">
-        <v>1407.2614046763103</v>
+        <v>1407.2608605798839</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>2770.626449954108</v>
+        <v>2770.6265071879297</v>
       </c>
       <c r="B12">
-        <v>2193.8781744486687</v>
+        <v>2201.7324782617106</v>
       </c>
       <c r="C12">
-        <v>1875.1042057517848</v>
+        <v>1896.5290666105197</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>2528.2387490187198</v>
+        <v>2528.2387483210841</v>
       </c>
       <c r="B13">
-        <v>1947.5466896032067</v>
+        <v>1947.5471764946674</v>
       </c>
       <c r="C13">
-        <v>1749.6330418674784</v>
+        <v>1749.6320391353865</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>2609.7077573395409</v>
+        <v>2609.7077576152847</v>
       </c>
       <c r="B14">
-        <v>2018.5468677722945</v>
+        <v>2018.747131381228</v>
       </c>
       <c r="C14">
-        <v>1759.5597087708768</v>
+        <v>1757.4978996681295</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>2503.2297760451011</v>
+        <v>2503.2248039583947</v>
       </c>
       <c r="B15">
-        <v>2051.416880995745</v>
+        <v>2051.8787234510228</v>
       </c>
       <c r="C15">
-        <v>1833.0290098974242</v>
+        <v>1832.9544835080455</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>2592.3768062015702</v>
+        <v>2592.376243186462</v>
       </c>
       <c r="B16">
-        <v>1797.2456078784303</v>
+        <v>1799.9947305053117</v>
       </c>
       <c r="C16">
-        <v>1568.6528356072297</v>
+        <v>1571.4178997318688</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>2356.8601401089932</v>
+        <v>2356.8601378921621</v>
       </c>
       <c r="B17">
-        <v>1814.1836892896029</v>
+        <v>1814.183856138367</v>
       </c>
       <c r="C17">
-        <v>1709.7092249325049</v>
+        <v>1709.7084558778279</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>2615.491122412915</v>
+        <v>2616.1384098191234</v>
       </c>
       <c r="B18">
-        <v>2163.1508444250139</v>
+        <v>2161.0004518584929</v>
       </c>
       <c r="C18">
-        <v>2077.7982519417487</v>
+        <v>2088.9723595506885</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>2011.2261617487509</v>
+        <v>2011.2295767214825</v>
       </c>
       <c r="B19">
-        <v>2033.9335197896344</v>
+        <v>2033.9315696339561</v>
       </c>
       <c r="C19">
-        <v>1981.0698214975762</v>
+        <v>1981.0685119676493</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>2576.2845513363582</v>
+        <v>2576.2845538913493</v>
       </c>
       <c r="B20">
-        <v>1981.3717182002993</v>
+        <v>1981.4044547233398</v>
       </c>
       <c r="C20">
-        <v>1870.0558660754841</v>
+        <v>1869.9530479197674</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>2713.0802018334111</v>
+        <v>2713.0801992948718</v>
       </c>
       <c r="B21">
-        <v>2020.8570458484212</v>
+        <v>2020.856815124363</v>
       </c>
       <c r="C21">
-        <v>1980.6742375270492</v>
+        <v>1980.6745582119877</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>2569.5114395448936</v>
+        <v>2569.5114393257518</v>
       </c>
       <c r="B22">
-        <v>1982.4411079456511</v>
+        <v>1982.44279635917</v>
       </c>
       <c r="C22">
-        <v>1731.9360952080569</v>
+        <v>1731.9157297969646</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed FP and FL boundary conditions to what  they were before and got good looking figures
</commit_message>
<xml_diff>
--- a/AIC9parameters_hptoolbox_moredata.xlsx
+++ b/AIC9parameters_hptoolbox_moredata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E336764-4420-46F7-8A90-30CF35380784}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8232E859-D108-42DD-AFED-D2A97067AAC2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11325" xr2:uid="{39B4C127-F51D-4565-9B09-D204C61B9351}"/>
   </bookViews>
@@ -387,244 +387,244 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>2504.3641874528048</v>
+        <v>2504.3641875225248</v>
       </c>
       <c r="B1">
-        <v>1675.4872758024103</v>
+        <v>1675.4817733253944</v>
       </c>
       <c r="C1">
-        <v>1659.1694206955858</v>
+        <v>1659.175700557744</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2263.2649304931097</v>
+        <v>2262.5551341635014</v>
       </c>
       <c r="B2">
-        <v>1537.5578724368795</v>
+        <v>1502.7606434992442</v>
       </c>
       <c r="C2">
-        <v>1393.2740556789715</v>
+        <v>1376.2941818763427</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2560.3680387196541</v>
+        <v>2560.3680356691543</v>
       </c>
       <c r="B3">
-        <v>1740.6137032078921</v>
+        <v>1740.6138750621997</v>
       </c>
       <c r="C3">
-        <v>1579.1404065201828</v>
+        <v>1579.0404426421503</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2495.9933054598469</v>
+        <v>2494.2816724362074</v>
       </c>
       <c r="B4">
-        <v>1913.3276998137765</v>
+        <v>1886.0880077709817</v>
       </c>
       <c r="C4">
-        <v>1951.620215286079</v>
+        <v>1890.1705214780602</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2528.8045935782193</v>
+        <v>2528.8038651354173</v>
       </c>
       <c r="B5">
-        <v>1752.3685036322445</v>
+        <v>1752.8912484338457</v>
       </c>
       <c r="C5">
-        <v>1755.617454012624</v>
+        <v>1754.8834586714404</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2480.0542736911661</v>
+        <v>2478.7488923483206</v>
       </c>
       <c r="B6">
-        <v>1850.23187819243</v>
+        <v>1826.3368947729757</v>
       </c>
       <c r="C6">
-        <v>1930.686298371365</v>
+        <v>1881.3871662939919</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2397.2088804141163</v>
+        <v>2397.2088800618067</v>
       </c>
       <c r="B7">
-        <v>1848.4313192171414</v>
+        <v>1848.4308520432855</v>
       </c>
       <c r="C7">
-        <v>1675.6626888020246</v>
+        <v>1675.6638407780397</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2467.9969994687162</v>
+        <v>2467.996998375711</v>
       </c>
       <c r="B8">
-        <v>1930.0304952068079</v>
+        <v>1930.0307207430074</v>
       </c>
       <c r="C8">
-        <v>1785.2212237624467</v>
+        <v>1785.2198927447378</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2643.8787844459366</v>
+        <v>2643.8788680913858</v>
       </c>
       <c r="B9">
-        <v>1957.2149355131842</v>
+        <v>1943.4610312448535</v>
       </c>
       <c r="C9">
-        <v>1663.4754274722636</v>
+        <v>1635.4856174790666</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2394.9100079198947</v>
+        <v>2394.9108173457316</v>
       </c>
       <c r="B10">
-        <v>1513.0137755996332</v>
+        <v>1520.2078910823648</v>
       </c>
       <c r="C10">
-        <v>1430.9226292086887</v>
+        <v>1429.4701744687366</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>2163.0420354858652</v>
+        <v>2163.0433237002462</v>
       </c>
       <c r="B11">
-        <v>1575.4241850871933</v>
+        <v>1575.4311100229684</v>
       </c>
       <c r="C11">
-        <v>1407.2608605798839</v>
+        <v>1407.2570777772714</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>2770.6265071879297</v>
+        <v>2770.6264484910107</v>
       </c>
       <c r="B12">
-        <v>2201.7324782617106</v>
+        <v>2193.8789571331267</v>
       </c>
       <c r="C12">
-        <v>1896.5290666105197</v>
+        <v>1875.0922041911349</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>2528.2387483210841</v>
+        <v>2528.1018186655519</v>
       </c>
       <c r="B13">
-        <v>1947.5471764946674</v>
+        <v>1948.3587415276781</v>
       </c>
       <c r="C13">
-        <v>1749.6320391353865</v>
+        <v>1754.633454248107</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>2609.7077576152847</v>
+        <v>2609.7077573736137</v>
       </c>
       <c r="B14">
-        <v>2018.747131381228</v>
+        <v>2018.5644302498422</v>
       </c>
       <c r="C14">
-        <v>1757.4978996681295</v>
+        <v>1759.3304433006706</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>2503.2248039583947</v>
+        <v>2498.8845153969119</v>
       </c>
       <c r="B15">
-        <v>2051.8787234510228</v>
+        <v>2026.4017199517746</v>
       </c>
       <c r="C15">
-        <v>1832.9544835080455</v>
+        <v>1838.8582161258253</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>2592.376243186462</v>
+        <v>2592.3756000667886</v>
       </c>
       <c r="B16">
-        <v>1799.9947305053117</v>
+        <v>1796.2617606532046</v>
       </c>
       <c r="C16">
-        <v>1571.4178997318688</v>
+        <v>1554.7405201260492</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>2356.8601378921621</v>
+        <v>2355.9502413785494</v>
       </c>
       <c r="B17">
-        <v>1814.183856138367</v>
+        <v>1785.7963220480617</v>
       </c>
       <c r="C17">
-        <v>1709.7084558778279</v>
+        <v>1699.7042402819582</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>2616.1384098191234</v>
+        <v>2615.6965196820511</v>
       </c>
       <c r="B18">
-        <v>2161.0004518584929</v>
+        <v>2162.0331228077912</v>
       </c>
       <c r="C18">
-        <v>2088.9723595506885</v>
+        <v>2083.448066940392</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>2011.2295767214825</v>
+        <v>2011.2296828283734</v>
       </c>
       <c r="B19">
-        <v>2033.9315696339561</v>
+        <v>2033.9312076960384</v>
       </c>
       <c r="C19">
-        <v>1981.0685119676493</v>
+        <v>1981.0689856943163</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>2576.2845538913493</v>
+        <v>2576.2845482917992</v>
       </c>
       <c r="B20">
-        <v>1981.4044547233398</v>
+        <v>1981.3402408926472</v>
       </c>
       <c r="C20">
-        <v>1869.9530479197674</v>
+        <v>1870.1560410687173</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>2713.0801992948718</v>
+        <v>2713.0802000001959</v>
       </c>
       <c r="B21">
-        <v>2020.856815124363</v>
+        <v>2020.8570413855018</v>
       </c>
       <c r="C21">
-        <v>1980.6745582119877</v>
+        <v>1980.6742389564292</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>2569.5114393257518</v>
+        <v>2569.5114382281931</v>
       </c>
       <c r="B22">
-        <v>1982.44279635917</v>
+        <v>1982.4267725062407</v>
       </c>
       <c r="C22">
-        <v>1731.9157297969646</v>
+        <v>1732.1200200450439</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added the TSC with in_ex to the cell_data for easy analysis
</commit_message>
<xml_diff>
--- a/AIC9parameters_hptoolbox_moredata.xlsx
+++ b/AIC9parameters_hptoolbox_moredata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8232E859-D108-42DD-AFED-D2A97067AAC2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19DD1DAD-9F99-4AEC-ACE0-254612007C54}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11325" xr2:uid="{39B4C127-F51D-4565-9B09-D204C61B9351}"/>
+    <workbookView xWindow="1908" yWindow="1908" windowWidth="17280" windowHeight="9060" xr2:uid="{39B4C127-F51D-4565-9B09-D204C61B9351}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -377,15 +377,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98533C2B-DACF-4252-91C9-AC407CD24EE6}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C22"/>
+      <selection sqref="A1:C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>2504.3641875225248</v>
       </c>
@@ -396,7 +396,7 @@
         <v>1659.175700557744</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2262.5551341635014</v>
       </c>
@@ -407,7 +407,7 @@
         <v>1376.2941818763427</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2560.3680356691543</v>
       </c>
@@ -418,7 +418,7 @@
         <v>1579.0404426421503</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2494.2816724362074</v>
       </c>
@@ -429,7 +429,7 @@
         <v>1890.1705214780602</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2528.8038651354173</v>
       </c>
@@ -440,7 +440,7 @@
         <v>1754.8834586714404</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2478.7488923483206</v>
       </c>
@@ -451,7 +451,7 @@
         <v>1881.3871662939919</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2397.2088800618067</v>
       </c>
@@ -462,7 +462,7 @@
         <v>1675.6638407780397</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2467.996998375711</v>
       </c>
@@ -473,7 +473,7 @@
         <v>1785.2198927447378</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2643.8788680913858</v>
       </c>
@@ -484,7 +484,7 @@
         <v>1635.4856174790666</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2394.9108173457316</v>
       </c>
@@ -495,7 +495,7 @@
         <v>1429.4701744687366</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2163.0433237002462</v>
       </c>
@@ -506,7 +506,7 @@
         <v>1407.2570777772714</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2770.6264484910107</v>
       </c>
@@ -517,7 +517,7 @@
         <v>1875.0922041911349</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2528.1018186655519</v>
       </c>
@@ -528,7 +528,7 @@
         <v>1754.633454248107</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2609.7077573736137</v>
       </c>
@@ -539,7 +539,7 @@
         <v>1759.3304433006706</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2498.8845153969119</v>
       </c>
@@ -550,7 +550,7 @@
         <v>1838.8582161258253</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2592.3756000667886</v>
       </c>
@@ -561,7 +561,7 @@
         <v>1554.7405201260492</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2355.9502413785494</v>
       </c>
@@ -572,7 +572,7 @@
         <v>1699.7042402819582</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2615.6965196820511</v>
       </c>
@@ -583,7 +583,7 @@
         <v>2083.448066940392</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2011.2296828283734</v>
       </c>
@@ -594,7 +594,7 @@
         <v>1981.0689856943163</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2576.2845482917992</v>
       </c>
@@ -605,7 +605,7 @@
         <v>1870.1560410687173</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2713.0802000001959</v>
       </c>
@@ -616,7 +616,7 @@
         <v>1980.6742389564292</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2569.5114382281931</v>
       </c>
@@ -625,6 +625,17 @@
       </c>
       <c r="C22">
         <v>1732.1200200450439</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>2527.0553673936838</v>
+      </c>
+      <c r="B23">
+        <v>1675.9277600756905</v>
+      </c>
+      <c r="C23">
+        <v>1776.6481060779727</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Got 9 param images back
</commit_message>
<xml_diff>
--- a/AIC9parameters_hptoolbox_moredata.xlsx
+++ b/AIC9parameters_hptoolbox_moredata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19DD1DAD-9F99-4AEC-ACE0-254612007C54}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5ABBD16-9D02-4590-95D9-0AFDBF437A6D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1908" yWindow="1908" windowWidth="17280" windowHeight="9060" xr2:uid="{39B4C127-F51D-4565-9B09-D204C61B9351}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{39B4C127-F51D-4565-9B09-D204C61B9351}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -383,9 +383,9 @@
       <selection sqref="A1:C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>2504.3641875225248</v>
       </c>
@@ -396,7 +396,7 @@
         <v>1659.175700557744</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2262.5551341635014</v>
       </c>
@@ -407,7 +407,7 @@
         <v>1376.2941818763427</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2560.3680356691543</v>
       </c>
@@ -418,7 +418,7 @@
         <v>1579.0404426421503</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2494.2816724362074</v>
       </c>
@@ -429,7 +429,7 @@
         <v>1890.1705214780602</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2528.8038651354173</v>
       </c>
@@ -440,7 +440,7 @@
         <v>1754.8834586714404</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2478.7488923483206</v>
       </c>
@@ -451,7 +451,7 @@
         <v>1881.3871662939919</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2397.2088800618067</v>
       </c>
@@ -462,7 +462,7 @@
         <v>1675.6638407780397</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2467.996998375711</v>
       </c>
@@ -473,7 +473,7 @@
         <v>1785.2198927447378</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2643.8788680913858</v>
       </c>
@@ -484,7 +484,7 @@
         <v>1635.4856174790666</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2394.9108173457316</v>
       </c>
@@ -495,7 +495,7 @@
         <v>1429.4701744687366</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2163.0433237002462</v>
       </c>
@@ -506,7 +506,7 @@
         <v>1407.2570777772714</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2770.6264484910107</v>
       </c>
@@ -517,7 +517,7 @@
         <v>1875.0922041911349</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2528.1018186655519</v>
       </c>
@@ -528,7 +528,7 @@
         <v>1754.633454248107</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2609.7077573736137</v>
       </c>
@@ -539,7 +539,7 @@
         <v>1759.3304433006706</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2498.8845153969119</v>
       </c>
@@ -550,7 +550,7 @@
         <v>1838.8582161258253</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2592.3756000667886</v>
       </c>
@@ -561,7 +561,7 @@
         <v>1554.7405201260492</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2355.9502413785494</v>
       </c>
@@ -572,7 +572,7 @@
         <v>1699.7042402819582</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2615.6965196820511</v>
       </c>
@@ -583,7 +583,7 @@
         <v>2083.448066940392</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2011.2296828283734</v>
       </c>
@@ -594,7 +594,7 @@
         <v>1981.0689856943163</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2576.2845482917992</v>
       </c>
@@ -605,7 +605,7 @@
         <v>1870.1560410687173</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2713.0802000001959</v>
       </c>
@@ -616,7 +616,7 @@
         <v>1980.6742389564292</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2569.5114382281931</v>
       </c>
@@ -627,7 +627,7 @@
         <v>1732.1200200450439</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2527.0553673936838</v>
       </c>

</xml_diff>